<commit_message>
Result Column added in datasheet
</commit_message>
<xml_diff>
--- a/TestData.xlsx
+++ b/TestData.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <workbookPr defaultThemeVersion="124226" filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView windowHeight="10740" windowWidth="14145" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Data" sheetId="1" r:id="rId1"/>
+    <sheet name="Data" r:id="rId1" sheetId="1"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="10">
   <si>
     <t xml:space="preserve">UserName </t>
   </si>
@@ -32,12 +33,25 @@
   </si>
   <si>
     <t>msdr97898</t>
+  </si>
+  <si>
+    <t>Results</t>
+  </si>
+  <si>
+    <t>Enter</t>
+  </si>
+  <si>
+    <t>PASS</t>
+  </si>
+  <si>
+    <t>FAIL</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -63,7 +77,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -71,19 +85,35 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+  <cellXfs count="3">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFont="1" borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleMedium9" defaultTableStyle="TableStyleMedium2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -100,10 +130,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -138,7 +168,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin panose="020F0302020204030204" typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -173,7 +203,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -261,7 +291,7 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="9525">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="95000"/>
@@ -270,13 +300,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="25400">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="38100">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -286,7 +316,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="20000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -295,7 +325,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -304,7 +334,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -314,12 +344,12 @@
             <a:camera prst="orthographicFront">
               <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig rig="threePt" dir="t">
+            <a:lightRig dir="t" rig="threePt">
               <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
-            <a:bevelT w="63500" h="25400"/>
+            <a:bevelT h="25400" w="63500"/>
           </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
@@ -350,7 +380,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+            <a:fillToRect b="180000" l="50000" r="50000" t="-80000"/>
           </a:path>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
@@ -369,7 +399,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+            <a:fillToRect b="50000" l="50000" r="50000" t="50000"/>
           </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
@@ -381,60 +411,66 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="W18" sqref="W18"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="11.28515625" customWidth="1"/>
+    <col min="1" max="2" customWidth="true" width="11.28515625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="C1" s="1" t="s">
+        <v>9</v>
+      </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="2" t="s">
         <v>3</v>
       </c>
+      <c r="C3" t="s">
+        <v>7</v>
+      </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="2" t="s">
         <v>5</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup orientation="portrait" paperSize="9" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>